<commit_message>
Spirit: updated performance measurements to use Boost.Format in an more efficient way
git-svn-id: http://svn.boost.org/svn/boost/trunk@54979 b8fc166d-592f-0410-95f2-cb63ce0dd405
</commit_message>
<xml_diff>
--- a/libs/spirit/doc/karma_performance.xlsx
+++ b/libs/spirit/doc/karma_performance.xlsx
@@ -11,9 +11,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -389,22 +386,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>9.2349999999999994</c:v>
+                  <c:v>3.1880000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0449999999999999</c:v>
+                  <c:v>3.7370000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.6189999999999998</c:v>
+                  <c:v>2.8780000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9219999999999997</c:v>
+                  <c:v>3.2170000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.75</c:v>
+                  <c:v>2.6720000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.35</c:v>
+                  <c:v>2.0110000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -479,11 +476,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="152"/>
-        <c:axId val="93557120"/>
-        <c:axId val="93558656"/>
+        <c:axId val="95703424"/>
+        <c:axId val="95704960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="93557120"/>
+        <c:axId val="95703424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -497,14 +494,14 @@
         </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93558656"/>
+        <c:crossAx val="95704960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93558656"/>
+        <c:axId val="95704960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -537,11 +534,10 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93557120"/>
+        <c:crossAx val="95703424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="2"/>
-        <c:minorUnit val="2"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:spPr>
         <a:ln w="12700">
@@ -604,7 +600,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000044" r="0.75000000000000044" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000056" r="0.75000000000000056" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -821,22 +817,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>9.2089999999999996</c:v>
+                  <c:v>6.0220000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.862</c:v>
+                  <c:v>6.8170000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.599</c:v>
+                  <c:v>5.7930000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.7100000000000009</c:v>
+                  <c:v>5.7210000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.11</c:v>
+                  <c:v>4.3540000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.9329999999999998</c:v>
+                  <c:v>4.0890000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -910,12 +906,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="95931008"/>
-        <c:axId val="98503296"/>
+        <c:axId val="96015488"/>
+        <c:axId val="96017024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="95931008"/>
+        <c:axId val="96015488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -929,17 +924,16 @@
         </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98503296"/>
+        <c:crossAx val="96017024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98503296"/>
+        <c:axId val="96017024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="12"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines>
@@ -970,7 +964,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95931008"/>
+        <c:crossAx val="96015488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1017,7 +1011,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1086,91 +1080,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Colors"/>
-      <sheetName val="Prelim"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="46">
-          <cell r="D46" t="str">
-            <v>Fills</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="B47" t="str">
-            <v>a</v>
-          </cell>
-          <cell r="D47">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="B48" t="str">
-            <v>b</v>
-          </cell>
-          <cell r="D48">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="B49" t="str">
-            <v>c</v>
-          </cell>
-          <cell r="D49">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="B50" t="str">
-            <v>d</v>
-          </cell>
-          <cell r="D50">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="B51" t="str">
-            <v>e</v>
-          </cell>
-          <cell r="D51">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="B52" t="str">
-            <v>f</v>
-          </cell>
-          <cell r="D52">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="B53" t="str">
-            <v>g</v>
-          </cell>
-          <cell r="D53">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="B54" t="str">
-            <v>h</v>
-          </cell>
-          <cell r="D54">
-            <v>4</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1460,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D3:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O49" sqref="O49"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39:J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1566,22 +1475,22 @@
         <v>2</v>
       </c>
       <c r="E6">
-        <v>9.2349999999999994</v>
+        <v>3.1880000000000002</v>
       </c>
       <c r="F6">
-        <v>8.0449999999999999</v>
+        <v>3.7370000000000001</v>
       </c>
       <c r="G6">
-        <v>6.6189999999999998</v>
+        <v>2.8780000000000001</v>
       </c>
       <c r="H6">
-        <v>5.9219999999999997</v>
+        <v>3.2170000000000001</v>
       </c>
       <c r="I6">
-        <v>5.75</v>
+        <v>2.6720000000000002</v>
       </c>
       <c r="J6">
-        <v>5.35</v>
+        <v>2.0110000000000001</v>
       </c>
       <c r="O6">
         <v>6.8879999999999999</v>
@@ -1795,22 +1704,22 @@
         <v>2</v>
       </c>
       <c r="E39">
-        <v>9.2089999999999996</v>
+        <v>6.0220000000000002</v>
       </c>
       <c r="F39">
-        <v>11.862</v>
+        <v>6.8170000000000002</v>
       </c>
       <c r="G39">
-        <v>10.599</v>
+        <v>5.7930000000000001</v>
       </c>
       <c r="H39">
-        <v>9.7100000000000009</v>
+        <v>5.7210000000000001</v>
       </c>
       <c r="I39">
-        <v>9.11</v>
+        <v>4.3540000000000001</v>
       </c>
       <c r="J39">
-        <v>7.9329999999999998</v>
+        <v>4.0890000000000004</v>
       </c>
       <c r="O39">
         <v>11.308</v>

</xml_diff>

<commit_message>
Spirit: benchmark and doc updates
git-svn-id: http://svn.boost.org/svn/boost/trunk@55019 b8fc166d-592f-0410-95f2-cb63ce0dd405
</commit_message>
<xml_diff>
--- a/libs/spirit/doc/karma_performance.xlsx
+++ b/libs/spirit/doc/karma_performance.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="24855" windowHeight="12780"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="24855" windowHeight="12780" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Single double" sheetId="1" r:id="rId1"/>
+    <sheet name="Sequence of items" sheetId="2" r:id="rId2"/>
+    <sheet name="Single int" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
   <si>
     <t xml:space="preserve">iostreams   </t>
   </si>
@@ -62,6 +63,12 @@
   <si>
     <t xml:space="preserve">sprintf        </t>
   </si>
+  <si>
+    <t>Converting 10000000 randomly generated int values to strings.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ltoa </t>
+  </si>
 </sst>
 </file>
 
@@ -96,8 +103,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -217,7 +227,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$4</c:f>
+              <c:f>'Single double'!$D$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -228,7 +238,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$3:$J$3</c:f>
+              <c:f>'Single double'!$E$3:$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -254,7 +264,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$4:$J$4</c:f>
+              <c:f>'Single double'!$E$4:$J$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -285,7 +295,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$5</c:f>
+              <c:f>'Single double'!$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -296,7 +306,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$3:$J$3</c:f>
+              <c:f>'Single double'!$E$3:$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -322,7 +332,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$J$5</c:f>
+              <c:f>'Single double'!$E$5:$J$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -353,7 +363,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$6</c:f>
+              <c:f>'Single double'!$D$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -364,7 +374,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$3:$J$3</c:f>
+              <c:f>'Single double'!$E$3:$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -390,7 +400,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$6:$J$6</c:f>
+              <c:f>'Single double'!$E$6:$J$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -421,7 +431,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$7</c:f>
+              <c:f>'Single double'!$D$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -432,7 +442,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$3:$J$3</c:f>
+              <c:f>'Single double'!$E$3:$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -458,7 +468,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$7:$J$7</c:f>
+              <c:f>'Single double'!$E$7:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -485,11 +495,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="152"/>
-        <c:axId val="98860032"/>
-        <c:axId val="98878208"/>
+        <c:axId val="88499328"/>
+        <c:axId val="88500864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="98860032"/>
+        <c:axId val="88499328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -503,14 +513,14 @@
         </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98878208"/>
+        <c:crossAx val="88500864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98878208"/>
+        <c:axId val="88500864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -543,7 +553,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98860032"/>
+        <c:crossAx val="88499328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -609,7 +619,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000078" r="0.75000000000000078" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.750000000000001" r="0.750000000000001" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -700,7 +710,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$37</c:f>
+              <c:f>'Sequence of items'!$D$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -711,7 +721,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$36:$J$36</c:f>
+              <c:f>'Sequence of items'!$E$3:$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -737,7 +747,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$37:$J$37</c:f>
+              <c:f>'Sequence of items'!$E$4:$J$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -768,7 +778,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$38</c:f>
+              <c:f>'Sequence of items'!$D$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -779,7 +789,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$36:$J$36</c:f>
+              <c:f>'Sequence of items'!$E$3:$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -805,7 +815,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$38:$J$38</c:f>
+              <c:f>'Sequence of items'!$E$5:$J$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -836,7 +846,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$39</c:f>
+              <c:f>'Sequence of items'!$D$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -847,7 +857,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$36:$J$36</c:f>
+              <c:f>'Sequence of items'!$E$3:$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -873,7 +883,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$39:$J$39</c:f>
+              <c:f>'Sequence of items'!$E$6:$J$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -904,7 +914,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$40</c:f>
+              <c:f>'Sequence of items'!$D$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -915,7 +925,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$36:$J$36</c:f>
+              <c:f>'Sequence of items'!$E$3:$J$3</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -941,7 +951,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$40:$J$40</c:f>
+              <c:f>'Sequence of items'!$E$7:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -967,11 +977,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="98642176"/>
-        <c:axId val="98652160"/>
+        <c:axId val="88535424"/>
+        <c:axId val="88536960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="98642176"/>
+        <c:axId val="88535424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -985,14 +995,14 @@
         </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98652160"/>
+        <c:crossAx val="88536960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98652160"/>
+        <c:axId val="88536960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1025,7 +1035,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98642176"/>
+        <c:crossAx val="88535424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1072,7 +1082,446 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Format single int</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>(10000000 iterations)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Single int'!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ltoa </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Single int'!$E$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>gcc 4.4.0 (32)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>VC++ 10 (32)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Intel 11.1 (32)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gcc 4.4.0 (64)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>VC++ 10 (64)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Intel 11.1 (64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Single int'!$E$4:$J$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.5589999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.85899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1180000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.88900000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Single int'!$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iostreams   </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Single int'!$E$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>gcc 4.4.0 (32)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>VC++ 10 (32)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Intel 11.1 (32)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gcc 4.4.0 (64)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>VC++ 10 (64)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Intel 11.1 (64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Single int'!$E$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.484</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.161</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.635999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.8120000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.3680000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Single int'!$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Boost.Format</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Single int'!$E$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>gcc 4.4.0 (32)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>VC++ 10 (32)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Intel 11.1 (32)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gcc 4.4.0 (64)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>VC++ 10 (64)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Intel 11.1 (64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Single int'!$E$6:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>16.823</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.568999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.706</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.401999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.222</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Single int'!$D$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Karma</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Single int'!$E$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>gcc 4.4.0 (32)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>VC++ 10 (32)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Intel 11.1 (32)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gcc 4.4.0 (64)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>VC++ 10 (64)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Intel 11.1 (64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Single int'!$E$7:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.5619999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0109999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.956</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.878</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="152"/>
+        <c:axId val="89719552"/>
+        <c:axId val="89721088"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="89719552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="89721088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="89721088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1050"/>
+                  <a:t>Measured time [s]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="89719552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx2"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent1">
+        <a:lumMod val="20000"/>
+        <a:lumOff val="80000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+    <a:effectLst>
+      <a:outerShdw blurRad="50800" dist="50800" dir="2700000" algn="tl" rotWithShape="0">
+        <a:prstClr val="black">
+          <a:alpha val="40000"/>
+        </a:prstClr>
+      </a:outerShdw>
+    </a:effectLst>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter alignWithMargins="0"/>
+    <c:pageMargins b="1" l="0.75000000000000122" r="0.75000000000000122" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1084,12 +1533,12 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>28573</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
@@ -1110,22 +1559,27 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>581024</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1134,7 +1588,42 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1428,15 +1917,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D3:P42"/>
+  <dimension ref="D3:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
@@ -1676,206 +2165,6 @@
         <v>0.254</v>
       </c>
     </row>
-    <row r="36" spans="4:16">
-      <c r="E36" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" t="s">
-        <v>10</v>
-      </c>
-      <c r="H36" t="s">
-        <v>11</v>
-      </c>
-      <c r="I36" t="s">
-        <v>12</v>
-      </c>
-      <c r="J36" t="s">
-        <v>13</v>
-      </c>
-      <c r="O36" t="s">
-        <v>5</v>
-      </c>
-      <c r="P36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="4:16">
-      <c r="D37" t="s">
-        <v>14</v>
-      </c>
-      <c r="E37">
-        <v>1.5249999999999999</v>
-      </c>
-      <c r="F37">
-        <v>1.9890000000000001</v>
-      </c>
-      <c r="G37">
-        <v>1.9319999999999999</v>
-      </c>
-      <c r="H37">
-        <v>1.4650000000000001</v>
-      </c>
-      <c r="I37">
-        <v>1.6930000000000001</v>
-      </c>
-      <c r="J37">
-        <v>1.532</v>
-      </c>
-      <c r="O37">
-        <v>2.0579999999999998</v>
-      </c>
-      <c r="P37">
-        <v>1.742</v>
-      </c>
-    </row>
-    <row r="38" spans="4:16">
-      <c r="D38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>4.5919999999999996</v>
-      </c>
-      <c r="F38">
-        <v>5.2939999999999996</v>
-      </c>
-      <c r="G38">
-        <v>4.367</v>
-      </c>
-      <c r="H38">
-        <v>3.1309999999999998</v>
-      </c>
-      <c r="I38">
-        <v>3.2719999999999998</v>
-      </c>
-      <c r="J38">
-        <v>2.762</v>
-      </c>
-      <c r="O38">
-        <v>4.1660000000000004</v>
-      </c>
-      <c r="P38">
-        <v>2.2229999999999999</v>
-      </c>
-    </row>
-    <row r="39" spans="4:16">
-      <c r="D39" t="s">
-        <v>1</v>
-      </c>
-      <c r="E39">
-        <v>6.0220000000000002</v>
-      </c>
-      <c r="F39">
-        <v>6.8170000000000002</v>
-      </c>
-      <c r="G39">
-        <v>5.7930000000000001</v>
-      </c>
-      <c r="H39">
-        <v>5.7210000000000001</v>
-      </c>
-      <c r="I39">
-        <v>4.3540000000000001</v>
-      </c>
-      <c r="J39">
-        <v>4.0890000000000004</v>
-      </c>
-      <c r="O39">
-        <v>11.308</v>
-      </c>
-      <c r="P39">
-        <v>5.1459999999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="4:16">
-      <c r="D40" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40">
-        <v>4.585</v>
-      </c>
-      <c r="F40">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="G40">
-        <v>3.5289999999999999</v>
-      </c>
-      <c r="H40">
-        <v>3.97</v>
-      </c>
-      <c r="I40">
-        <v>1.5920000000000001</v>
-      </c>
-      <c r="J40">
-        <v>1.8129999999999999</v>
-      </c>
-      <c r="O40">
-        <v>4.3659999999999997</v>
-      </c>
-      <c r="P40">
-        <v>1.867</v>
-      </c>
-    </row>
-    <row r="41" spans="4:16">
-      <c r="D41" t="s">
-        <v>2</v>
-      </c>
-      <c r="E41">
-        <v>4.7130000000000001</v>
-      </c>
-      <c r="F41">
-        <v>2.972</v>
-      </c>
-      <c r="G41">
-        <v>5.3760000000000003</v>
-      </c>
-      <c r="H41">
-        <v>4.0510000000000002</v>
-      </c>
-      <c r="I41">
-        <v>2.024</v>
-      </c>
-      <c r="J41">
-        <v>2.7730000000000001</v>
-      </c>
-      <c r="O41">
-        <v>6.5</v>
-      </c>
-      <c r="P41">
-        <v>1.6579999999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="4:16">
-      <c r="D42" t="s">
-        <v>3</v>
-      </c>
-      <c r="E42">
-        <v>4.5810000000000004</v>
-      </c>
-      <c r="F42">
-        <v>2.5790000000000002</v>
-      </c>
-      <c r="G42">
-        <v>3.5329999999999999</v>
-      </c>
-      <c r="H42">
-        <v>4.1619999999999999</v>
-      </c>
-      <c r="I42">
-        <v>1.5740000000000001</v>
-      </c>
-      <c r="J42">
-        <v>1.7509999999999999</v>
-      </c>
-      <c r="O42">
-        <v>4.3440000000000003</v>
-      </c>
-      <c r="P42">
-        <v>1.893</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1884,24 +2173,372 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="D3:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:16">
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="4:16">
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>1.5249999999999999</v>
+      </c>
+      <c r="F4">
+        <v>1.9890000000000001</v>
+      </c>
+      <c r="G4">
+        <v>1.9319999999999999</v>
+      </c>
+      <c r="H4">
+        <v>1.4650000000000001</v>
+      </c>
+      <c r="I4">
+        <v>1.6930000000000001</v>
+      </c>
+      <c r="J4">
+        <v>1.532</v>
+      </c>
+      <c r="O4">
+        <v>2.0579999999999998</v>
+      </c>
+      <c r="P4">
+        <v>1.742</v>
+      </c>
+    </row>
+    <row r="5" spans="4:16">
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>4.5919999999999996</v>
+      </c>
+      <c r="F5">
+        <v>5.2939999999999996</v>
+      </c>
+      <c r="G5">
+        <v>4.367</v>
+      </c>
+      <c r="H5">
+        <v>3.1309999999999998</v>
+      </c>
+      <c r="I5">
+        <v>3.2719999999999998</v>
+      </c>
+      <c r="J5">
+        <v>2.762</v>
+      </c>
+      <c r="O5">
+        <v>4.1660000000000004</v>
+      </c>
+      <c r="P5">
+        <v>2.2229999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="4:16">
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>6.0220000000000002</v>
+      </c>
+      <c r="F6">
+        <v>6.8170000000000002</v>
+      </c>
+      <c r="G6">
+        <v>5.7930000000000001</v>
+      </c>
+      <c r="H6">
+        <v>5.7210000000000001</v>
+      </c>
+      <c r="I6">
+        <v>4.3540000000000001</v>
+      </c>
+      <c r="J6">
+        <v>4.0890000000000004</v>
+      </c>
+      <c r="O6">
+        <v>11.308</v>
+      </c>
+      <c r="P6">
+        <v>5.1459999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="4:16">
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>4.585</v>
+      </c>
+      <c r="F7">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="G7">
+        <v>3.5289999999999999</v>
+      </c>
+      <c r="H7">
+        <v>3.97</v>
+      </c>
+      <c r="I7">
+        <v>1.5920000000000001</v>
+      </c>
+      <c r="J7">
+        <v>1.8129999999999999</v>
+      </c>
+      <c r="O7">
+        <v>4.3659999999999997</v>
+      </c>
+      <c r="P7">
+        <v>1.867</v>
+      </c>
+    </row>
+    <row r="8" spans="4:16">
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>4.7130000000000001</v>
+      </c>
+      <c r="F8">
+        <v>2.972</v>
+      </c>
+      <c r="G8">
+        <v>5.3760000000000003</v>
+      </c>
+      <c r="H8">
+        <v>4.0510000000000002</v>
+      </c>
+      <c r="I8">
+        <v>2.024</v>
+      </c>
+      <c r="J8">
+        <v>2.7730000000000001</v>
+      </c>
+      <c r="O8">
+        <v>6.5</v>
+      </c>
+      <c r="P8">
+        <v>1.6579999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="4:16">
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>4.5810000000000004</v>
+      </c>
+      <c r="F9">
+        <v>2.5790000000000002</v>
+      </c>
+      <c r="G9">
+        <v>3.5329999999999999</v>
+      </c>
+      <c r="H9">
+        <v>4.1619999999999999</v>
+      </c>
+      <c r="I9">
+        <v>1.5740000000000001</v>
+      </c>
+      <c r="J9">
+        <v>1.7509999999999999</v>
+      </c>
+      <c r="O9">
+        <v>4.3440000000000003</v>
+      </c>
+      <c r="P9">
+        <v>1.893</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="D1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7:P10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:10">
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="4:10">
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="4:10">
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>1.5589999999999999</v>
+      </c>
+      <c r="F4">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="G4">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="H4">
+        <v>1.2</v>
+      </c>
+      <c r="I4">
+        <v>1.1180000000000001</v>
+      </c>
+      <c r="J4">
+        <v>0.88900000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="4:10">
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>6.484</v>
+      </c>
+      <c r="F5">
+        <v>13.161</v>
+      </c>
+      <c r="G5">
+        <v>11.635999999999999</v>
+      </c>
+      <c r="H5">
+        <v>3.42</v>
+      </c>
+      <c r="I5">
+        <v>7.8120000000000003</v>
+      </c>
+      <c r="J5">
+        <v>7.3680000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="4:10">
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>16.823</v>
+      </c>
+      <c r="F6">
+        <v>21.568999999999999</v>
+      </c>
+      <c r="G6">
+        <v>19.706</v>
+      </c>
+      <c r="H6">
+        <v>17.28</v>
+      </c>
+      <c r="I6">
+        <v>14.401999999999999</v>
+      </c>
+      <c r="J6">
+        <v>13.222</v>
+      </c>
+    </row>
+    <row r="7" spans="4:10">
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>2.5619999999999998</v>
+      </c>
+      <c r="F7">
+        <v>1.0109999999999999</v>
+      </c>
+      <c r="G7">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="H7">
+        <v>2.956</v>
+      </c>
+      <c r="I7">
+        <v>1.016</v>
+      </c>
+      <c r="J7">
+        <v>0.878</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10">
+      <c r="E12" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Spirit: added one more Karma benchmark
git-svn-id: http://svn.boost.org/svn/boost/trunk@55025 b8fc166d-592f-0410-95f2-cb63ce0dd405
</commit_message>
<xml_diff>
--- a/libs/spirit/doc/karma_performance.xlsx
+++ b/libs/spirit/doc/karma_performance.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="24855" windowHeight="12780" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="24855" windowHeight="12780" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Single double" sheetId="1" r:id="rId1"/>
     <sheet name="Sequence of items" sheetId="2" r:id="rId2"/>
     <sheet name="Single int" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
   <si>
     <t xml:space="preserve">iostreams   </t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t xml:space="preserve">ltoa </t>
+  </si>
+  <si>
+    <t>Benchmarking sequence of different length:</t>
+  </si>
+  <si>
+    <t>VC8SP1</t>
   </si>
 </sst>
 </file>
@@ -495,11 +501,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="152"/>
-        <c:axId val="88499328"/>
-        <c:axId val="88500864"/>
+        <c:axId val="93536640"/>
+        <c:axId val="93538176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88499328"/>
+        <c:axId val="93536640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -513,14 +519,14 @@
         </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88500864"/>
+        <c:crossAx val="93538176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88500864"/>
+        <c:axId val="93538176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -553,7 +559,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88499328"/>
+        <c:crossAx val="93536640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -619,7 +625,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.750000000000001" r="0.750000000000001" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000111" r="0.75000000000000111" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -977,11 +983,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="88535424"/>
-        <c:axId val="88536960"/>
+        <c:axId val="94015488"/>
+        <c:axId val="94017024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88535424"/>
+        <c:axId val="94015488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -995,14 +1001,14 @@
         </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88536960"/>
+        <c:crossAx val="94017024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88536960"/>
+        <c:axId val="94017024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1035,7 +1041,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88535424"/>
+        <c:crossAx val="94015488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1082,7 +1088,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1398,11 +1404,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="152"/>
-        <c:axId val="89719552"/>
-        <c:axId val="89721088"/>
+        <c:axId val="94090752"/>
+        <c:axId val="94092288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89719552"/>
+        <c:axId val="94090752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1416,14 +1422,14 @@
         </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89721088"/>
+        <c:crossAx val="94092288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89721088"/>
+        <c:axId val="94092288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1456,7 +1462,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89719552"/>
+        <c:crossAx val="94090752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1521,7 +1527,679 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000122" r="0.75000000000000122" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000133" r="0.75000000000000133" t="1" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Karma sequences</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>(10000000 iterations)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>gcc 4.4.0 (32)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$5:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.627</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.298</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9059999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4780000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6760000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.9449999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>VC++ 10 (32)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$5:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.42399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.49199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2170000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7889999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.986</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5129999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.8290000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.7320000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Intel 11.1 (32)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$5:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.56899999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.448</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9890000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5960000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.242</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5590000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.2460000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>gcc 4.4.0 (64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$5:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.81899999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2769999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.472</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2290000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7090000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2050000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.3769999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5920000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>VC++ 10 (64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$5:$K$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.311</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.441</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.76800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6339999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.853</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Intel 11.1 (64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$5:$L$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.42599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.69499999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0189999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6339999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.008</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3239999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.6619999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="152"/>
+        <c:axId val="58122624"/>
+        <c:axId val="58124160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="58122624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1050"/>
+                  <a:t>Sequence length (elements)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="58124160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="58124160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1050"/>
+                  <a:t>Measured time [s]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="58122624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx2"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent1">
+        <a:lumMod val="20000"/>
+        <a:lumOff val="80000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+    <a:effectLst>
+      <a:outerShdw blurRad="50800" dist="50800" dir="2700000" algn="tl" rotWithShape="0">
+        <a:prstClr val="black">
+          <a:alpha val="40000"/>
+        </a:prstClr>
+      </a:outerShdw>
+    </a:effectLst>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter alignWithMargins="0"/>
+    <c:pageMargins b="1" l="0.75000000000000155" r="0.75000000000000155" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1611,6 +2289,41 @@
       <xdr:colOff>590550</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2402,8 +3115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7:P10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2541,4 +3254,265 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="E1:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:12">
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="5:12">
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="5:12">
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="G5">
+        <v>0.627</v>
+      </c>
+      <c r="H5">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="I5">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="J5">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="K5">
+        <v>0.311</v>
+      </c>
+      <c r="L5">
+        <v>0.42599999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="5:12">
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>0.7</v>
+      </c>
+      <c r="G6">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="H6">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="I6">
+        <v>0.98</v>
+      </c>
+      <c r="J6">
+        <v>1.2769999999999999</v>
+      </c>
+      <c r="K6">
+        <v>0.441</v>
+      </c>
+      <c r="L6">
+        <v>0.69499999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="5:12">
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>1.044</v>
+      </c>
+      <c r="G7">
+        <v>1.298</v>
+      </c>
+      <c r="H7">
+        <v>1.2170000000000001</v>
+      </c>
+      <c r="I7">
+        <v>1.448</v>
+      </c>
+      <c r="J7">
+        <v>1.472</v>
+      </c>
+      <c r="K7">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="L7">
+        <v>1.0189999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="5:12">
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>1.4430000000000001</v>
+      </c>
+      <c r="G8">
+        <v>1.65</v>
+      </c>
+      <c r="H8">
+        <v>1.7889999999999999</v>
+      </c>
+      <c r="I8">
+        <v>1.9890000000000001</v>
+      </c>
+      <c r="J8">
+        <v>2.2290000000000001</v>
+      </c>
+      <c r="K8">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="L8">
+        <v>1.2649999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="5:12">
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>1.76</v>
+      </c>
+      <c r="G9">
+        <v>1.9059999999999999</v>
+      </c>
+      <c r="H9">
+        <v>1.986</v>
+      </c>
+      <c r="I9">
+        <v>2.5960000000000001</v>
+      </c>
+      <c r="J9">
+        <v>2.7090000000000001</v>
+      </c>
+      <c r="K9">
+        <v>1.216</v>
+      </c>
+      <c r="L9">
+        <v>1.6339999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="5:12">
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>2.214</v>
+      </c>
+      <c r="G10">
+        <v>2.4780000000000002</v>
+      </c>
+      <c r="H10">
+        <v>2.5129999999999999</v>
+      </c>
+      <c r="I10">
+        <v>3.242</v>
+      </c>
+      <c r="J10">
+        <v>3.2050000000000001</v>
+      </c>
+      <c r="K10">
+        <v>1.6339999999999999</v>
+      </c>
+      <c r="L10">
+        <v>2.008</v>
+      </c>
+    </row>
+    <row r="11" spans="5:12">
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>2.7559999999999998</v>
+      </c>
+      <c r="G11">
+        <v>2.6760000000000002</v>
+      </c>
+      <c r="H11">
+        <v>2.8290000000000002</v>
+      </c>
+      <c r="I11">
+        <v>3.5590000000000002</v>
+      </c>
+      <c r="J11">
+        <v>3.3769999999999998</v>
+      </c>
+      <c r="K11">
+        <v>1.853</v>
+      </c>
+      <c r="L11">
+        <v>2.3239999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="5:12">
+      <c r="E12">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <v>3.29</v>
+      </c>
+      <c r="G12">
+        <v>2.9449999999999998</v>
+      </c>
+      <c r="H12">
+        <v>3.7320000000000002</v>
+      </c>
+      <c r="I12">
+        <v>4.2460000000000004</v>
+      </c>
+      <c r="J12">
+        <v>3.5920000000000001</v>
+      </c>
+      <c r="K12">
+        <v>2.11</v>
+      </c>
+      <c r="L12">
+        <v>2.6619999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Spirit: improving overall performance, doc update
git-svn-id: http://svn.boost.org/svn/boost/trunk@55035 b8fc166d-592f-0410-95f2-cb63ce0dd405
</commit_message>
<xml_diff>
--- a/libs/spirit/doc/karma_performance.xlsx
+++ b/libs/spirit/doc/karma_performance.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="24855" windowHeight="12780" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="24855" windowHeight="12780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Single double" sheetId="1" r:id="rId1"/>
     <sheet name="Sequence of items" sheetId="2" r:id="rId2"/>
     <sheet name="Single int" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sequence" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="19">
   <si>
     <t xml:space="preserve">iostreams   </t>
   </si>
@@ -221,7 +221,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -501,11 +500,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="152"/>
-        <c:axId val="93536640"/>
-        <c:axId val="93538176"/>
+        <c:axId val="96617216"/>
+        <c:axId val="96618752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="93536640"/>
+        <c:axId val="96617216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -519,14 +518,14 @@
         </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93538176"/>
+        <c:crossAx val="96618752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93538176"/>
+        <c:axId val="96618752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -554,12 +553,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93536640"/>
+        <c:crossAx val="96617216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -581,7 +579,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -625,7 +622,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000111" r="0.75000000000000111" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000133" r="0.75000000000000133" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -758,22 +755,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.5249999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.9890000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.9319999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.4650000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.6930000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.532</c:v>
+                  <c:v>1.7250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8919999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.903</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6080000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4930000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -826,22 +823,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.5919999999999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.2939999999999996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.367</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.1309999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.2719999999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.762</c:v>
+                  <c:v>4.827</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2869999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.444</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1120000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.319</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.8769999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -894,22 +891,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.0220000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.8170000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.7930000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.7210000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.3540000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.0890000000000004</c:v>
+                  <c:v>5.8810000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0890000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8010000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.4550000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.2539999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.1639999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -962,32 +959,32 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.585</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.4500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.5289999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.97</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.5920000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.8129999999999999</c:v>
+                  <c:v>1.9419999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.242</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3340000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.75800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68600000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="94015488"/>
-        <c:axId val="94017024"/>
+        <c:axId val="97759616"/>
+        <c:axId val="97761152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="94015488"/>
+        <c:axId val="97759616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1001,14 +998,14 @@
         </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94017024"/>
+        <c:crossAx val="97761152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94017024"/>
+        <c:axId val="97761152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1041,7 +1038,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94015488"/>
+        <c:crossAx val="97759616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1088,7 +1085,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1124,7 +1121,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1404,11 +1400,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="152"/>
-        <c:axId val="94090752"/>
-        <c:axId val="94092288"/>
+        <c:axId val="97830784"/>
+        <c:axId val="97832320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="94090752"/>
+        <c:axId val="97830784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1422,14 +1418,684 @@
         </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94092288"/>
+        <c:crossAx val="97832320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94092288"/>
+        <c:axId val="97832320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1050"/>
+                  <a:t>Measured time [s]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="97830784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx2"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent1">
+        <a:lumMod val="20000"/>
+        <a:lumOff val="80000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+    <a:effectLst>
+      <a:outerShdw blurRad="50800" dist="50800" dir="2700000" algn="tl" rotWithShape="0">
+        <a:prstClr val="black">
+          <a:alpha val="40000"/>
+        </a:prstClr>
+      </a:outerShdw>
+    </a:effectLst>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter alignWithMargins="0"/>
+    <c:pageMargins b="1" l="0.75000000000000155" r="0.75000000000000155" t="1" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Karma sequences</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>(10000000 iterations)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sequence!$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>gcc 4.4.0 (32)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sequence!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sequence!$G$5:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.48399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.69699999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.095</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.248</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.456</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6879999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7290000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sequence!$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>VC++ 10 (32)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sequence!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sequence!$H$5:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.20499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.41399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.65800000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.877</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.335</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sequence!$I$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Intel 11.1 (32)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sequence!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sequence!$I$5:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.41599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.54600000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.81599999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.052</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3080000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.849</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0670000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4350000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sequence!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>gcc 4.4.0 (64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sequence!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sequence!$J$5:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.68300000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.034</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3480000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7070000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.363</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.498</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sequence!$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>VC++ 10 (64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sequence!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sequence!$K$5:$K$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.16500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.46500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.71699999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.82799999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.93400000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sequence!$L$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Intel 11.1 (64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sequence!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sequence!$L$5:$L$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.27500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.439</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.628</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.88100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2849999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.351</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7090000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="152"/>
+        <c:axId val="98189312"/>
+        <c:axId val="98191232"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="98189312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1050"/>
+                  <a:t>Sequence length (elements)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98191232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="98191232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1462,7 +2128,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94090752"/>
+        <c:crossAx val="98189312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1527,13 +2193,13 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000133" r="0.75000000000000133" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000178" r="0.75000000000000178" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:style val="18"/>
@@ -1549,7 +2215,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Karma sequences</a:t>
+              <a:t>Karma sequences (plain output iterator)</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -1575,7 +2241,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$4</c:f>
+              <c:f>Sequence!$Q$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1586,7 +2252,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$12</c:f>
+              <c:f>Sequence!$E$5:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1619,33 +2285,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$5:$G$12</c:f>
+              <c:f>Sequence!$Q$5:$Q$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.627</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.95599999999999996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.298</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.65</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.9059999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.4780000000000002</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.9000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.105</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.6760000000000002</c:v>
+                  <c:v>0.13500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.9449999999999998</c:v>
+                  <c:v>0.20399999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1656,7 +2322,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$4</c:f>
+              <c:f>Sequence!$R$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1667,7 +2333,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$12</c:f>
+              <c:f>Sequence!$E$5:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1700,33 +2366,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$5:$H$12</c:f>
+              <c:f>Sequence!$R$5:$R$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.42399999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.49199999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.2170000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.7889999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.986</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.5129999999999999</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.48499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.72099999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.8290000000000002</c:v>
+                  <c:v>0.86499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.7320000000000002</c:v>
+                  <c:v>1.075</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1737,7 +2403,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$4</c:f>
+              <c:f>Sequence!$S$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1748,7 +2414,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$12</c:f>
+              <c:f>Sequence!$E$5:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1781,33 +2447,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$5:$I$12</c:f>
+              <c:f>Sequence!$S$5:$S$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.56899999999999995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.98</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.448</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.9890000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.5960000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.242</c:v>
+                  <c:v>0.26300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.38700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.501</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.66800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.90200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.153</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5590000000000002</c:v>
+                  <c:v>1.423</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.2460000000000004</c:v>
+                  <c:v>1.728</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1818,7 +2484,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$4</c:f>
+              <c:f>Sequence!$T$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1829,7 +2495,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$12</c:f>
+              <c:f>Sequence!$E$5:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1862,33 +2528,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$5:$J$12</c:f>
+              <c:f>Sequence!$T$5:$T$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.81899999999999995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.2769999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.472</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.2290000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.7090000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.2050000000000001</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.2000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3769999999999998</c:v>
+                  <c:v>0.14499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5920000000000001</c:v>
+                  <c:v>0.16300000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1899,7 +2565,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$4</c:f>
+              <c:f>Sequence!$U$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1910,7 +2576,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$12</c:f>
+              <c:f>Sequence!$E$5:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1943,33 +2609,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$5:$K$12</c:f>
+              <c:f>Sequence!$U$5:$U$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.311</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.441</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.76800000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.97499999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.216</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.6339999999999999</c:v>
+                  <c:v>7.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.853</c:v>
+                  <c:v>0.49199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.11</c:v>
+                  <c:v>0.58799999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1980,7 +2646,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$4</c:f>
+              <c:f>Sequence!$V$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1991,7 +2657,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$12</c:f>
+              <c:f>Sequence!$E$5:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2024,44 +2690,44 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$5:$L$12</c:f>
+              <c:f>Sequence!$V$5:$V$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.42599999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.69499999999999995</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0189999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2649999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.6339999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.008</c:v>
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.30499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.52700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3239999999999998</c:v>
+                  <c:v>0.82699999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.6619999999999999</c:v>
+                  <c:v>0.97099999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:gapWidth val="152"/>
-        <c:axId val="58122624"/>
-        <c:axId val="58124160"/>
+        <c:axId val="78198272"/>
+        <c:axId val="78200192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58122624"/>
+        <c:axId val="78198272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2094,14 +2760,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58124160"/>
+        <c:crossAx val="78200192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58124160"/>
+        <c:axId val="78200192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2134,9 +2800,10 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58122624"/>
+        <c:crossAx val="78198272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:spPr>
         <a:ln w="12700">
@@ -2199,7 +2866,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000155" r="0.75000000000000155" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.750000000000002" r="0.750000000000002" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2337,6 +3004,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2888,8 +3585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D3:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2936,25 +3633,25 @@
         <v>14</v>
       </c>
       <c r="E4">
-        <v>1.5249999999999999</v>
+        <v>1.7250000000000001</v>
       </c>
       <c r="F4">
-        <v>1.9890000000000001</v>
+        <v>1.8919999999999999</v>
       </c>
       <c r="G4">
-        <v>1.9319999999999999</v>
+        <v>1.903</v>
       </c>
       <c r="H4">
-        <v>1.4650000000000001</v>
+        <v>1.4690000000000001</v>
       </c>
       <c r="I4">
-        <v>1.6930000000000001</v>
+        <v>1.6080000000000001</v>
       </c>
       <c r="J4">
-        <v>1.532</v>
+        <v>1.4930000000000001</v>
       </c>
       <c r="O4">
-        <v>2.0579999999999998</v>
+        <v>1.917</v>
       </c>
       <c r="P4">
         <v>1.742</v>
@@ -2965,25 +3662,25 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>4.5919999999999996</v>
+        <v>4.827</v>
       </c>
       <c r="F5">
-        <v>5.2939999999999996</v>
+        <v>5.2869999999999999</v>
       </c>
       <c r="G5">
-        <v>4.367</v>
+        <v>4.444</v>
       </c>
       <c r="H5">
-        <v>3.1309999999999998</v>
+        <v>3.1120000000000001</v>
       </c>
       <c r="I5">
-        <v>3.2719999999999998</v>
+        <v>3.319</v>
       </c>
       <c r="J5">
-        <v>2.762</v>
+        <v>2.8769999999999998</v>
       </c>
       <c r="O5">
-        <v>4.1660000000000004</v>
+        <v>4.1440000000000001</v>
       </c>
       <c r="P5">
         <v>2.2229999999999999</v>
@@ -2994,25 +3691,25 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>6.0220000000000002</v>
+        <v>5.8810000000000002</v>
       </c>
       <c r="F6">
-        <v>6.8170000000000002</v>
+        <v>7.0890000000000004</v>
       </c>
       <c r="G6">
-        <v>5.7930000000000001</v>
+        <v>5.8010000000000002</v>
       </c>
       <c r="H6">
-        <v>5.7210000000000001</v>
+        <v>5.4550000000000001</v>
       </c>
       <c r="I6">
-        <v>4.3540000000000001</v>
+        <v>5.2539999999999996</v>
       </c>
       <c r="J6">
-        <v>4.0890000000000004</v>
+        <v>4.1639999999999997</v>
       </c>
       <c r="O6">
-        <v>11.308</v>
+        <v>6.0960000000000001</v>
       </c>
       <c r="P6">
         <v>5.1459999999999999</v>
@@ -3023,25 +3720,25 @@
         <v>7</v>
       </c>
       <c r="E7">
-        <v>4.585</v>
+        <v>1.9419999999999999</v>
       </c>
       <c r="F7">
-        <v>2.4500000000000002</v>
+        <v>1.242</v>
       </c>
       <c r="G7">
-        <v>3.5289999999999999</v>
+        <v>0.999</v>
       </c>
       <c r="H7">
-        <v>3.97</v>
+        <v>1.3340000000000001</v>
       </c>
       <c r="I7">
-        <v>1.5920000000000001</v>
+        <v>0.75800000000000001</v>
       </c>
       <c r="J7">
-        <v>1.8129999999999999</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="O7">
-        <v>4.3659999999999997</v>
+        <v>1.143</v>
       </c>
       <c r="P7">
         <v>1.867</v>
@@ -3052,25 +3749,25 @@
         <v>2</v>
       </c>
       <c r="E8">
-        <v>4.7130000000000001</v>
+        <v>2.2429999999999999</v>
       </c>
       <c r="F8">
-        <v>2.972</v>
+        <v>1.728</v>
       </c>
       <c r="G8">
-        <v>5.3760000000000003</v>
+        <v>2.9119999999999999</v>
       </c>
       <c r="H8">
-        <v>4.0510000000000002</v>
+        <v>1.4119999999999999</v>
       </c>
       <c r="I8">
-        <v>2.024</v>
+        <v>1.1519999999999999</v>
       </c>
       <c r="J8">
-        <v>2.7730000000000001</v>
+        <v>1.365</v>
       </c>
       <c r="O8">
-        <v>6.5</v>
+        <v>3.3639999999999999</v>
       </c>
       <c r="P8">
         <v>1.6579999999999999</v>
@@ -3081,25 +3778,25 @@
         <v>3</v>
       </c>
       <c r="E9">
-        <v>4.5810000000000004</v>
+        <v>1.998</v>
       </c>
       <c r="F9">
-        <v>2.5790000000000002</v>
+        <v>1.25</v>
       </c>
       <c r="G9">
-        <v>3.5329999999999999</v>
+        <v>1.0149999999999999</v>
       </c>
       <c r="H9">
-        <v>4.1619999999999999</v>
+        <v>1.2989999999999999</v>
       </c>
       <c r="I9">
-        <v>1.5740000000000001</v>
+        <v>0.76900000000000002</v>
       </c>
       <c r="J9">
-        <v>1.7509999999999999</v>
+        <v>0.55100000000000005</v>
       </c>
       <c r="O9">
-        <v>4.3440000000000003</v>
+        <v>1.25</v>
       </c>
       <c r="P9">
         <v>1.893</v>
@@ -3258,10 +3955,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="E1:L12"/>
+  <dimension ref="E1:V12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3273,14 +3970,20 @@
     <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:12">
+    <row r="1" spans="5:22">
       <c r="E1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="5:12">
+    <row r="4" spans="5:22">
       <c r="F4" t="s">
         <v>18</v>
       </c>
@@ -3302,213 +4005,402 @@
       <c r="L4" t="s">
         <v>13</v>
       </c>
+      <c r="P4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S4" t="s">
+        <v>10</v>
+      </c>
+      <c r="T4" t="s">
+        <v>11</v>
+      </c>
+      <c r="U4" t="s">
+        <v>12</v>
+      </c>
+      <c r="V4" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="5" spans="5:12">
+    <row r="5" spans="5:22">
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5">
-        <v>0.25600000000000001</v>
+        <v>0.17</v>
       </c>
       <c r="G5">
-        <v>0.627</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="H5">
-        <v>0.42399999999999999</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="I5">
-        <v>0.56899999999999995</v>
+        <v>0.41599999999999998</v>
       </c>
       <c r="J5">
-        <v>0.81899999999999995</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="K5">
-        <v>0.311</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="L5">
-        <v>0.42599999999999999</v>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="P5">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="S5">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="V5">
+        <v>0.14699999999999999</v>
       </c>
     </row>
-    <row r="6" spans="5:12">
+    <row r="6" spans="5:22">
       <c r="E6">
         <v>3</v>
       </c>
       <c r="F6">
-        <v>0.7</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="G6">
-        <v>0.95599999999999996</v>
+        <v>0.69699999999999995</v>
       </c>
       <c r="H6">
-        <v>0.49199999999999999</v>
+        <v>0.23899999999999999</v>
       </c>
       <c r="I6">
-        <v>0.98</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="J6">
-        <v>1.2769999999999999</v>
+        <v>1.034</v>
       </c>
       <c r="K6">
-        <v>0.441</v>
+        <v>0.21099999999999999</v>
       </c>
       <c r="L6">
-        <v>0.69499999999999995</v>
+        <v>0.439</v>
+      </c>
+      <c r="P6">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="Q6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="R6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="S6">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="T6">
+        <v>0.02</v>
+      </c>
+      <c r="U6">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="V6">
+        <v>0.24199999999999999</v>
       </c>
     </row>
-    <row r="7" spans="5:12">
+    <row r="7" spans="5:22">
       <c r="E7">
         <v>4</v>
       </c>
       <c r="F7">
-        <v>1.044</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="G7">
-        <v>1.298</v>
+        <v>0.89300000000000002</v>
       </c>
       <c r="H7">
-        <v>1.2170000000000001</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="I7">
-        <v>1.448</v>
+        <v>0.81599999999999995</v>
       </c>
       <c r="J7">
-        <v>1.472</v>
+        <v>1.3480000000000001</v>
       </c>
       <c r="K7">
-        <v>0.76800000000000002</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="L7">
-        <v>1.0189999999999999</v>
+        <v>0.628</v>
+      </c>
+      <c r="P7">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="Q7">
+        <v>3.1E-2</v>
+      </c>
+      <c r="R7">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="S7">
+        <v>0.501</v>
+      </c>
+      <c r="T7">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="U7">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="V7">
+        <v>0.30499999999999999</v>
       </c>
     </row>
-    <row r="8" spans="5:12">
+    <row r="8" spans="5:22">
       <c r="E8">
         <v>5</v>
       </c>
       <c r="F8">
-        <v>1.4430000000000001</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="G8">
-        <v>1.65</v>
+        <v>1.095</v>
       </c>
       <c r="H8">
-        <v>1.7889999999999999</v>
+        <v>0.61499999999999999</v>
       </c>
       <c r="I8">
-        <v>1.9890000000000001</v>
+        <v>1.052</v>
       </c>
       <c r="J8">
-        <v>2.2290000000000001</v>
+        <v>1.7070000000000001</v>
       </c>
       <c r="K8">
-        <v>0.97499999999999998</v>
+        <v>0.39900000000000002</v>
       </c>
       <c r="L8">
-        <v>1.2649999999999999</v>
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="P8">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="Q8">
+        <v>5.5E-2</v>
+      </c>
+      <c r="R8">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="S8">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="T8">
+        <v>0.06</v>
+      </c>
+      <c r="U8">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="V8">
+        <v>0.53</v>
       </c>
     </row>
-    <row r="9" spans="5:12">
+    <row r="9" spans="5:22">
       <c r="E9">
         <v>6</v>
       </c>
       <c r="F9">
-        <v>1.76</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="G9">
-        <v>1.9059999999999999</v>
+        <v>1.248</v>
       </c>
       <c r="H9">
-        <v>1.986</v>
+        <v>0.65800000000000003</v>
       </c>
       <c r="I9">
-        <v>2.5960000000000001</v>
+        <v>1.3080000000000001</v>
       </c>
       <c r="J9">
-        <v>2.7090000000000001</v>
+        <v>2.008</v>
       </c>
       <c r="K9">
-        <v>1.216</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="L9">
-        <v>1.6339999999999999</v>
+        <v>1.008</v>
+      </c>
+      <c r="P9">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="Q9">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="R9">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="S9">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="T9">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="U9">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="V9">
+        <v>0.52700000000000002</v>
       </c>
     </row>
-    <row r="10" spans="5:12">
+    <row r="10" spans="5:22">
       <c r="E10">
         <v>7</v>
       </c>
       <c r="F10">
-        <v>2.214</v>
+        <v>0.82799999999999996</v>
       </c>
       <c r="G10">
-        <v>2.4780000000000002</v>
+        <v>1.456</v>
       </c>
       <c r="H10">
-        <v>2.5129999999999999</v>
+        <v>0.877</v>
       </c>
       <c r="I10">
-        <v>3.242</v>
+        <v>1.849</v>
       </c>
       <c r="J10">
-        <v>3.2050000000000001</v>
+        <v>2.363</v>
       </c>
       <c r="K10">
-        <v>1.6339999999999999</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="L10">
-        <v>2.008</v>
+        <v>1.2849999999999999</v>
+      </c>
+      <c r="P10">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="Q10">
+        <v>0.105</v>
+      </c>
+      <c r="R10">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="S10">
+        <v>1.153</v>
+      </c>
+      <c r="T10">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="U10">
+        <v>0.42</v>
+      </c>
+      <c r="V10">
+        <v>0.61299999999999999</v>
       </c>
     </row>
-    <row r="11" spans="5:12">
+    <row r="11" spans="5:22">
       <c r="E11">
         <v>8</v>
       </c>
       <c r="F11">
-        <v>2.7559999999999998</v>
+        <v>1.153</v>
       </c>
       <c r="G11">
-        <v>2.6760000000000002</v>
+        <v>1.6879999999999999</v>
       </c>
       <c r="H11">
-        <v>2.8290000000000002</v>
+        <v>0.98099999999999998</v>
       </c>
       <c r="I11">
-        <v>3.5590000000000002</v>
+        <v>2.0670000000000002</v>
       </c>
       <c r="J11">
-        <v>3.3769999999999998</v>
+        <v>1.498</v>
       </c>
       <c r="K11">
-        <v>1.853</v>
+        <v>0.82799999999999996</v>
       </c>
       <c r="L11">
-        <v>2.3239999999999998</v>
+        <v>1.351</v>
+      </c>
+      <c r="P11">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="Q11">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="R11">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="S11">
+        <v>1.423</v>
+      </c>
+      <c r="T11">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="U11">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="V11">
+        <v>0.82699999999999996</v>
       </c>
     </row>
-    <row r="12" spans="5:12">
+    <row r="12" spans="5:22">
       <c r="E12">
         <v>9</v>
       </c>
       <c r="F12">
-        <v>3.29</v>
+        <v>1.333</v>
       </c>
       <c r="G12">
-        <v>2.9449999999999998</v>
+        <v>1.7290000000000001</v>
       </c>
       <c r="H12">
-        <v>3.7320000000000002</v>
+        <v>1.335</v>
       </c>
       <c r="I12">
-        <v>4.2460000000000004</v>
+        <v>2.4350000000000001</v>
       </c>
       <c r="J12">
-        <v>3.5920000000000001</v>
+        <v>3.101</v>
       </c>
       <c r="K12">
-        <v>2.11</v>
+        <v>0.93400000000000005</v>
       </c>
       <c r="L12">
-        <v>2.6619999999999999</v>
+        <v>1.7090000000000001</v>
+      </c>
+      <c r="P12">
+        <v>1.024</v>
+      </c>
+      <c r="Q12">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="R12">
+        <v>1.075</v>
+      </c>
+      <c r="S12">
+        <v>1.728</v>
+      </c>
+      <c r="T12">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="U12">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="V12">
+        <v>0.97099999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Spirit: new performance data, updated docs
git-svn-id: http://svn.boost.org/svn/boost/trunk@55072 b8fc166d-592f-0410-95f2-cb63ce0dd405
</commit_message>
<xml_diff>
--- a/libs/spirit/doc/karma_performance.xlsx
+++ b/libs/spirit/doc/karma_performance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="24855" windowHeight="12780"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="24855" windowHeight="12780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Single double" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="22">
   <si>
     <t xml:space="preserve">iostreams   </t>
   </si>
@@ -74,6 +74,15 @@
   </si>
   <si>
     <t>VC8SP1</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>using fusion cons</t>
+  </si>
+  <si>
+    <t>using fusion vector</t>
   </si>
 </sst>
 </file>
@@ -221,7 +230,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -501,11 +509,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="152"/>
-        <c:axId val="82793216"/>
-        <c:axId val="82794752"/>
+        <c:axId val="96767360"/>
+        <c:axId val="96785536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82793216"/>
+        <c:axId val="96767360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -519,14 +527,14 @@
         </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82794752"/>
+        <c:crossAx val="96785536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82794752"/>
+        <c:axId val="96785536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -554,12 +562,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82793216"/>
+        <c:crossAx val="96767360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -581,7 +588,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -625,7 +631,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000144" r="0.75000000000000144" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000167" r="0.75000000000000167" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -704,7 +710,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -983,11 +988,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="83149184"/>
-        <c:axId val="83150720"/>
+        <c:axId val="96295936"/>
+        <c:axId val="96314112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="83149184"/>
+        <c:axId val="96295936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1001,14 +1006,14 @@
         </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83150720"/>
+        <c:crossAx val="96314112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83150720"/>
+        <c:axId val="96314112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1036,12 +1041,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83149184"/>
+        <c:crossAx val="96295936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1062,7 +1066,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1088,7 +1091,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1178,22 +1181,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.5589999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.88100000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.85899999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.1180000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.88900000000000001</c:v>
+                  <c:v>1.542</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.163</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.099</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.90600000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1246,22 +1249,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6.484</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13.161</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.635999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.42</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.8120000000000003</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.3680000000000003</c:v>
+                  <c:v>6.548</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.727</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.898</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.464</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.3160000000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1150000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1314,22 +1317,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>16.823</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>21.568999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>19.706</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17.28</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.401999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13.222</c:v>
+                  <c:v>16.998000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.812999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.477</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.463999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.662000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.646000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1382,33 +1385,33 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.5619999999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0109999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.95499999999999996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.956</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.016</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.878</c:v>
+                  <c:v>1.421</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.74399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69699999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0720000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.95299999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.60599999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:gapWidth val="152"/>
-        <c:axId val="83478400"/>
-        <c:axId val="83479936"/>
+        <c:axId val="98497280"/>
+        <c:axId val="98498816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="83478400"/>
+        <c:axId val="98497280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1422,14 +1425,14 @@
         </c:majorGridlines>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83479936"/>
+        <c:crossAx val="98498816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83479936"/>
+        <c:axId val="98498816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1462,679 +1465,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83478400"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx2"/>
-          </a:solidFill>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="50800" dir="2700000" algn="tl" rotWithShape="0">
-            <a:prstClr val="black">
-              <a:alpha val="40000"/>
-            </a:prstClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="accent1">
-        <a:lumMod val="20000"/>
-        <a:lumOff val="80000"/>
-      </a:schemeClr>
-    </a:solidFill>
-    <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx2"/>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-    </a:ln>
-    <a:effectLst>
-      <a:outerShdw blurRad="50800" dist="50800" dir="2700000" algn="tl" rotWithShape="0">
-        <a:prstClr val="black">
-          <a:alpha val="40000"/>
-        </a:prstClr>
-      </a:outerShdw>
-    </a:effectLst>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr>
-          <a:solidFill>
-            <a:schemeClr val="dk1"/>
-          </a:solidFill>
-          <a:latin typeface="+mn-lt"/>
-          <a:ea typeface="+mn-ea"/>
-          <a:cs typeface="+mn-cs"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000167" r="0.75000000000000167" t="1" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:style val="18"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Karma sequences</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>(10000000 iterations)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sequence!$G$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>gcc 4.4.0 (32)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sequence!$E$5:$E$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sequence!$G$5:$G$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.48399999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.69699999999999995</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.89300000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.095</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.248</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.456</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.6879999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.7290000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sequence!$H$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>VC++ 10 (32)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sequence!$E$5:$E$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sequence!$H$5:$H$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.20499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.23899999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.41399999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.61499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.65800000000000003</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.877</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.98099999999999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.335</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sequence!$I$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Intel 11.1 (32)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sequence!$E$5:$E$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sequence!$I$5:$I$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.41599999999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.54600000000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.81599999999999995</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.052</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.3080000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.849</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.0670000000000002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.4350000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sequence!$J$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>gcc 4.4.0 (64)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sequence!$E$5:$E$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sequence!$J$5:$J$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.68300000000000005</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.034</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.3480000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.7070000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.008</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.363</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.498</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.101</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sequence!$K$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>VC++ 10 (64)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sequence!$E$5:$E$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sequence!$K$5:$K$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.16500000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.21099999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.33600000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.39900000000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.46500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.71699999999999997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.82799999999999996</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.93400000000000005</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sequence!$L$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Intel 11.1 (64)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sequence!$E$5:$E$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sequence!$L$5:$L$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.27500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.439</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.628</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.88100000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.008</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.2849999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.351</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.7090000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:gapWidth val="152"/>
-        <c:axId val="85680128"/>
-        <c:axId val="85682048"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="85680128"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:prstDash val="sysDot"/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1050"/>
-                  <a:t>Sequence length (elements)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85682048"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="85682048"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:prstDash val="sysDot"/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1050"/>
-                  <a:t>Measured time [s]</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85680128"/>
+        <c:crossAx val="98497280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2205,7 +1536,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:style val="18"/>
@@ -2221,7 +1552,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Karma sequences (plain output iterator)</a:t>
+              <a:t>Karma sequences</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -2247,7 +1578,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sequence!$Q$4</c:f>
+              <c:f>Sequence!$G$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2291,7 +1622,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sequence!$Q$5:$Q$12</c:f>
+              <c:f>Sequence!$G$5:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2299,25 +1630,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.1E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.5E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.9000000000000006E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.105</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.5999999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.13500000000000001</c:v>
+                  <c:v>0.114</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.20399999999999999</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2328,7 +1659,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sequence!$R$4</c:f>
+              <c:f>Sequence!$H$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2372,33 +1703,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sequence!$R$5:$R$12</c:f>
+              <c:f>Sequence!$H$5:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>8.9999999999999993E-3</c:v>
+                  <c:v>8.0000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.2999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.45700000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.48499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.63800000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.72099999999999997</c:v>
+                  <c:v>0.34699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.41099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.86499999999999999</c:v>
+                  <c:v>0.64100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.075</c:v>
+                  <c:v>0.93899999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2409,7 +1740,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sequence!$S$4</c:f>
+              <c:f>Sequence!$I$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2453,33 +1784,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sequence!$S$5:$S$12</c:f>
+              <c:f>Sequence!$I$5:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.26300000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.38700000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.501</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.66800000000000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.90200000000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.153</c:v>
+                  <c:v>0.22500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.69599999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.93899999999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.097</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.423</c:v>
+                  <c:v>1.254</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.728</c:v>
+                  <c:v>1.591</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2490,7 +1821,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sequence!$T$4</c:f>
+              <c:f>Sequence!$J$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2534,7 +1865,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sequence!$T$5:$T$12</c:f>
+              <c:f>Sequence!$J$5:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2542,25 +1873,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.02</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.3000000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.2000000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.11600000000000001</c:v>
+                <c:pt idx="4">
+                  <c:v>5.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.5999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.14499999999999999</c:v>
+                  <c:v>8.7999999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16300000000000001</c:v>
+                  <c:v>0.11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2571,7 +1902,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sequence!$U$4</c:f>
+              <c:f>Sequence!$K$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2615,33 +1946,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sequence!$U$5:$U$12</c:f>
+              <c:f>Sequence!$K$5:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>7.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.27400000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.34399999999999997</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.45300000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.42</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.30499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.49199999999999999</c:v>
+                  <c:v>0.57399999999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.58799999999999997</c:v>
+                  <c:v>0.57599999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2652,7 +1983,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sequence!$V$4</c:f>
+              <c:f>Sequence!$L$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2696,44 +2027,44 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sequence!$V$5:$V$12</c:f>
+              <c:f>Sequence!$L$5:$L$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.14699999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.24199999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.30499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.53</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.52700000000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.61299999999999999</c:v>
+                  <c:v>0.10199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.189</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.57999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.82699999999999996</c:v>
+                  <c:v>0.69199999999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.97099999999999997</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:gapWidth val="152"/>
-        <c:axId val="85727104"/>
-        <c:axId val="85737472"/>
+        <c:axId val="98519680"/>
+        <c:axId val="98525952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="85727104"/>
+        <c:axId val="98519680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2766,16 +2097,17 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85737472"/>
+        <c:crossAx val="98525952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85737472"/>
+        <c:axId val="98525952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines>
@@ -2806,7 +2138,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85727104"/>
+        <c:crossAx val="98519680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -2873,6 +2205,708 @@
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
     <c:pageMargins b="1" l="0.75000000000000211" r="0.75000000000000211" t="1" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Karma sequences (as_vector)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>(</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0" smtClean="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>10000000</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t> iterations)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sequence!$Q$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>gcc 4.4.0 (32)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sequence!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sequence!$Q$5:$Q$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.7000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.188</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.185</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14099999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sequence!$R$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>VC++ 10 (32)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sequence!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sequence!$R$5:$R$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.36699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.46500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.69699999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.745</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0920000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sequence!$S$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Intel 11.1 (32)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sequence!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sequence!$S$5:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.17199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.376</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.115</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.53</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sequence!$T$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>gcc 4.4.0 (64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sequence!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sequence!$T$5:$T$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.3999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.5999999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sequence!$U$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>VC++ 10 (64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sequence!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sequence!$U$5:$U$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.34100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.433</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.54900000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sequence!$V$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Intel 11.1 (64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sequence!$E$5:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sequence!$V$5:$V$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.10299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.34499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.52100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.60099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="152"/>
+        <c:axId val="98562816"/>
+        <c:axId val="98564736"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="98562816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1050"/>
+                  <a:t>Sequence length (elements)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98564736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="98564736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1050"/>
+                  <a:t>Measured time [s]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98562816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx2"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="2700000" algn="tl" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent1">
+        <a:lumMod val="20000"/>
+        <a:lumOff val="80000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+    <a:effectLst>
+      <a:outerShdw blurRad="50800" dist="50800" dir="2700000" algn="tl" rotWithShape="0">
+        <a:prstClr val="black">
+          <a:alpha val="40000"/>
+        </a:prstClr>
+      </a:outerShdw>
+    </a:effectLst>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter alignWithMargins="0"/>
+    <c:pageMargins b="1" l="0.75000000000000233" r="0.75000000000000233" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3335,7 +3369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D3:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I4" sqref="I4:I10"/>
     </sheetView>
   </sheetViews>
@@ -3818,8 +3852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3863,22 +3897,22 @@
         <v>16</v>
       </c>
       <c r="E4">
-        <v>1.5589999999999999</v>
+        <v>1.542</v>
       </c>
       <c r="F4">
-        <v>0.88100000000000001</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="G4">
-        <v>0.85899999999999999</v>
+        <v>0.88400000000000001</v>
       </c>
       <c r="H4">
-        <v>1.2</v>
+        <v>1.163</v>
       </c>
       <c r="I4">
-        <v>1.1180000000000001</v>
+        <v>1.099</v>
       </c>
       <c r="J4">
-        <v>0.88900000000000001</v>
+        <v>0.90600000000000003</v>
       </c>
     </row>
     <row r="5" spans="4:10">
@@ -3886,22 +3920,22 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>6.484</v>
+        <v>6.548</v>
       </c>
       <c r="F5">
-        <v>13.161</v>
+        <v>13.727</v>
       </c>
       <c r="G5">
-        <v>11.635999999999999</v>
+        <v>11.898</v>
       </c>
       <c r="H5">
-        <v>3.42</v>
+        <v>3.464</v>
       </c>
       <c r="I5">
-        <v>7.8120000000000003</v>
+        <v>8.3160000000000007</v>
       </c>
       <c r="J5">
-        <v>7.3680000000000003</v>
+        <v>8.1150000000000002</v>
       </c>
     </row>
     <row r="6" spans="4:10">
@@ -3909,22 +3943,22 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>16.823</v>
+        <v>16.998000000000001</v>
       </c>
       <c r="F6">
-        <v>21.568999999999999</v>
+        <v>21.812999999999999</v>
       </c>
       <c r="G6">
-        <v>19.706</v>
+        <v>20.477</v>
       </c>
       <c r="H6">
-        <v>17.28</v>
+        <v>17.463999999999999</v>
       </c>
       <c r="I6">
-        <v>14.401999999999999</v>
+        <v>14.662000000000001</v>
       </c>
       <c r="J6">
-        <v>13.222</v>
+        <v>13.646000000000001</v>
       </c>
     </row>
     <row r="7" spans="4:10">
@@ -3932,22 +3966,22 @@
         <v>7</v>
       </c>
       <c r="E7">
-        <v>2.5619999999999998</v>
+        <v>1.421</v>
       </c>
       <c r="F7">
-        <v>1.0109999999999999</v>
+        <v>0.74399999999999999</v>
       </c>
       <c r="G7">
-        <v>0.95499999999999996</v>
+        <v>0.69699999999999995</v>
       </c>
       <c r="H7">
-        <v>2.956</v>
+        <v>1.0720000000000001</v>
       </c>
       <c r="I7">
-        <v>1.016</v>
+        <v>0.95299999999999996</v>
       </c>
       <c r="J7">
-        <v>0.878</v>
+        <v>0.60599999999999998</v>
       </c>
     </row>
     <row r="12" spans="4:10">
@@ -3963,8 +3997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="E1:V12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:J12"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3978,10 +4012,9 @@
     <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="5:22">
@@ -3989,7 +4022,18 @@
         <v>17</v>
       </c>
     </row>
+    <row r="3" spans="5:22">
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="4" spans="5:22">
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
       <c r="F4" t="s">
         <v>18</v>
       </c>
@@ -4038,46 +4082,46 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <v>0.17</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="G5">
-        <v>0.48399999999999999</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.20499999999999999</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="I5">
-        <v>0.41599999999999998</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="J5">
-        <v>0.68300000000000005</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>0.16500000000000001</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="L5">
-        <v>0.27500000000000002</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="P5">
-        <v>8.0000000000000002E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5">
-        <v>8.9999999999999993E-3</v>
+        <v>0.01</v>
       </c>
       <c r="S5">
-        <v>0.26300000000000001</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="T5">
         <v>0</v>
       </c>
       <c r="U5">
-        <v>7.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="V5">
-        <v>0.14699999999999999</v>
+        <v>0.10299999999999999</v>
       </c>
     </row>
     <row r="6" spans="5:22">
@@ -4085,46 +4129,46 @@
         <v>3</v>
       </c>
       <c r="F6">
-        <v>0.20399999999999999</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="G6">
-        <v>0.69699999999999995</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>0.23899999999999999</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="I6">
-        <v>0.54600000000000004</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="J6">
-        <v>1.034</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>0.21099999999999999</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="L6">
-        <v>0.439</v>
+        <v>0.189</v>
       </c>
       <c r="P6">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="Q6">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="R6">
+        <v>1.4E-2</v>
+      </c>
+      <c r="S6">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="S6">
-        <v>0.38700000000000001</v>
-      </c>
-      <c r="T6">
-        <v>0.02</v>
-      </c>
-      <c r="U6">
-        <v>1.0999999999999999E-2</v>
-      </c>
       <c r="V6">
-        <v>0.24199999999999999</v>
+        <v>0.26400000000000001</v>
       </c>
     </row>
     <row r="7" spans="5:22">
@@ -4132,46 +4176,46 @@
         <v>4</v>
       </c>
       <c r="F7">
-        <v>0.38500000000000001</v>
+        <v>0.159</v>
       </c>
       <c r="G7">
-        <v>0.89300000000000002</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H7">
-        <v>0.41399999999999998</v>
+        <v>0.34699999999999998</v>
       </c>
       <c r="I7">
-        <v>0.81599999999999995</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="J7">
-        <v>1.3480000000000001</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="K7">
-        <v>0.33600000000000002</v>
+        <v>1.9E-2</v>
       </c>
       <c r="L7">
-        <v>0.628</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="P7">
-        <v>0.36399999999999999</v>
+        <v>1.6E-2</v>
       </c>
       <c r="Q7">
-        <v>3.1E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="R7">
-        <v>0.45700000000000002</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="S7">
-        <v>0.501</v>
+        <v>0.376</v>
       </c>
       <c r="T7">
-        <v>3.3000000000000002E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="U7">
-        <v>0.27400000000000002</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="V7">
-        <v>0.30499999999999999</v>
+        <v>0.34499999999999997</v>
       </c>
     </row>
     <row r="8" spans="5:22">
@@ -4179,46 +4223,46 @@
         <v>5</v>
       </c>
       <c r="F8">
-        <v>0.55500000000000005</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="G8">
-        <v>1.095</v>
+        <v>1.2E-2</v>
       </c>
       <c r="H8">
-        <v>0.61499999999999999</v>
+        <v>0.35899999999999999</v>
       </c>
       <c r="I8">
-        <v>1.052</v>
+        <v>0.69599999999999995</v>
       </c>
       <c r="J8">
-        <v>1.7070000000000001</v>
+        <v>0.02</v>
       </c>
       <c r="K8">
-        <v>0.39900000000000002</v>
+        <v>2.7E-2</v>
       </c>
       <c r="L8">
-        <v>0.88100000000000001</v>
+        <v>0.34100000000000003</v>
       </c>
       <c r="P8">
-        <v>0.42599999999999999</v>
+        <v>0.216</v>
       </c>
       <c r="Q8">
-        <v>5.5E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="R8">
-        <v>0.48499999999999999</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="S8">
-        <v>0.66800000000000004</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="T8">
-        <v>0.06</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="U8">
-        <v>0.34399999999999997</v>
+        <v>0.20799999999999999</v>
       </c>
       <c r="V8">
-        <v>0.53</v>
+        <v>0.46200000000000002</v>
       </c>
     </row>
     <row r="9" spans="5:22">
@@ -4226,46 +4270,46 @@
         <v>6</v>
       </c>
       <c r="F9">
-        <v>0.66100000000000003</v>
+        <v>0.434</v>
       </c>
       <c r="G9">
-        <v>1.248</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="H9">
-        <v>0.65800000000000003</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="I9">
-        <v>1.3080000000000001</v>
+        <v>0.93899999999999995</v>
       </c>
       <c r="J9">
-        <v>2.008</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="K9">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="L9">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="P9">
+        <v>0.44</v>
+      </c>
+      <c r="Q9">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="R9">
         <v>0.46500000000000002</v>
       </c>
-      <c r="L9">
-        <v>1.008</v>
-      </c>
-      <c r="P9">
-        <v>0.52200000000000002</v>
-      </c>
-      <c r="Q9">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="R9">
-        <v>0.63800000000000001</v>
-      </c>
       <c r="S9">
-        <v>0.90200000000000002</v>
+        <v>0.83</v>
       </c>
       <c r="T9">
-        <v>8.2000000000000003E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="U9">
-        <v>0.45300000000000001</v>
+        <v>0.34100000000000003</v>
       </c>
       <c r="V9">
-        <v>0.52700000000000002</v>
+        <v>0.52100000000000002</v>
       </c>
     </row>
     <row r="10" spans="5:22">
@@ -4273,46 +4317,46 @@
         <v>7</v>
       </c>
       <c r="F10">
-        <v>0.82799999999999996</v>
+        <v>0.56499999999999995</v>
       </c>
       <c r="G10">
-        <v>1.456</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="H10">
-        <v>0.877</v>
+        <v>0.59</v>
       </c>
       <c r="I10">
-        <v>1.849</v>
+        <v>1.097</v>
       </c>
       <c r="J10">
-        <v>2.363</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="K10">
-        <v>0.71699999999999997</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="L10">
-        <v>1.2849999999999999</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="P10">
-        <v>0.64300000000000002</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="Q10">
-        <v>0.105</v>
+        <v>0.188</v>
       </c>
       <c r="R10">
-        <v>0.72099999999999997</v>
+        <v>0.69699999999999995</v>
       </c>
       <c r="S10">
-        <v>1.153</v>
+        <v>1.115</v>
       </c>
       <c r="T10">
-        <v>0.11600000000000001</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="U10">
-        <v>0.42</v>
+        <v>0.433</v>
       </c>
       <c r="V10">
-        <v>0.61299999999999999</v>
+        <v>0.60099999999999998</v>
       </c>
     </row>
     <row r="11" spans="5:22">
@@ -4320,46 +4364,46 @@
         <v>8</v>
       </c>
       <c r="F11">
-        <v>1.153</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="G11">
-        <v>1.6879999999999999</v>
+        <v>0.114</v>
       </c>
       <c r="H11">
-        <v>0.98099999999999998</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="I11">
-        <v>2.0670000000000002</v>
+        <v>1.254</v>
       </c>
       <c r="J11">
-        <v>1.498</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="K11">
-        <v>0.82799999999999996</v>
+        <v>0.57399999999999995</v>
       </c>
       <c r="L11">
-        <v>1.351</v>
+        <v>0.69199999999999995</v>
       </c>
       <c r="P11">
-        <v>0.90100000000000002</v>
+        <v>0.78300000000000003</v>
       </c>
       <c r="Q11">
-        <v>0.13500000000000001</v>
+        <v>0.185</v>
       </c>
       <c r="R11">
-        <v>0.86499999999999999</v>
+        <v>0.745</v>
       </c>
       <c r="S11">
-        <v>1.423</v>
+        <v>1.32</v>
       </c>
       <c r="T11">
-        <v>0.14499999999999999</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="U11">
-        <v>0.49199999999999999</v>
+        <v>0.48799999999999999</v>
       </c>
       <c r="V11">
-        <v>0.82699999999999996</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="12" spans="5:22">
@@ -4367,46 +4411,46 @@
         <v>9</v>
       </c>
       <c r="F12">
-        <v>1.333</v>
+        <v>0.89700000000000002</v>
       </c>
       <c r="G12">
-        <v>1.7290000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H12">
-        <v>1.335</v>
+        <v>0.93899999999999995</v>
       </c>
       <c r="I12">
-        <v>2.4350000000000001</v>
+        <v>1.591</v>
       </c>
       <c r="J12">
-        <v>3.101</v>
+        <v>0.11</v>
       </c>
       <c r="K12">
-        <v>0.93400000000000005</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="L12">
-        <v>1.7090000000000001</v>
+        <v>0.84</v>
       </c>
       <c r="P12">
-        <v>1.024</v>
+        <v>1.038</v>
       </c>
       <c r="Q12">
-        <v>0.20399999999999999</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="R12">
-        <v>1.075</v>
+        <v>1.0920000000000001</v>
       </c>
       <c r="S12">
-        <v>1.728</v>
+        <v>1.53</v>
       </c>
       <c r="T12">
-        <v>0.16300000000000001</v>
+        <v>0.11</v>
       </c>
       <c r="U12">
-        <v>0.58799999999999997</v>
+        <v>0.54900000000000004</v>
       </c>
       <c r="V12">
-        <v>0.97099999999999997</v>
+        <v>0.85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>